<commit_message>
Quantile_Regression and exporting Word file
</commit_message>
<xml_diff>
--- a/Mobility_data/Other_input/Table_Variables.xlsx
+++ b/Mobility_data/Other_input/Table_Variables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t>varname</t>
   </si>
@@ -158,9 +158,6 @@
     <t>0: not chosen / 1: chosen</t>
   </si>
   <si>
-    <t>attitude_toadd</t>
-  </si>
-  <si>
     <t>accessibility</t>
   </si>
   <si>
@@ -234,6 +231,24 @@
   </si>
   <si>
     <t>99: keine angabe</t>
+  </si>
+  <si>
+    <t>toadd_attitude</t>
+  </si>
+  <si>
+    <t>from 1 (täglich) bis 5 (nie bzw. Fast nie) / 9: keine Angabe</t>
+  </si>
+  <si>
+    <t>Frequency_Car</t>
+  </si>
+  <si>
+    <t>P_NUTZ_AUTO</t>
+  </si>
+  <si>
+    <t>Frequency_OPNV</t>
+  </si>
+  <si>
+    <t>P_NUTZ_OPNV</t>
   </si>
 </sst>
 </file>
@@ -558,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -586,7 +601,7 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -600,7 +615,7 @@
         <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -617,7 +632,7 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3">
         <v>11</v>
@@ -634,7 +649,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4">
         <v>6</v>
@@ -668,7 +683,7 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -685,7 +700,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -702,7 +717,7 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8">
         <v>11</v>
@@ -719,7 +734,7 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9">
         <v>9</v>
@@ -736,7 +751,7 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10">
         <v>9</v>
@@ -747,13 +762,13 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11">
         <v>9</v>
@@ -770,7 +785,7 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12">
         <v>9</v>
@@ -787,7 +802,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13">
         <v>9</v>
@@ -798,13 +813,13 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14">
         <v>9</v>
@@ -815,13 +830,13 @@
         <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15">
         <v>9</v>
@@ -838,7 +853,7 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16">
         <v>9</v>
@@ -852,7 +867,7 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
         <v>43</v>
@@ -869,10 +884,10 @@
         <v>24</v>
       </c>
       <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
         <v>45</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
       </c>
       <c r="E18">
         <v>9</v>
@@ -880,16 +895,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E19">
         <v>7</v>
@@ -897,16 +912,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20">
         <v>7</v>
@@ -914,16 +929,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
         <v>60</v>
-      </c>
-      <c r="B21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" t="s">
-        <v>61</v>
       </c>
       <c r="E21">
         <v>7</v>
@@ -931,16 +946,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
         <v>63</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" t="s">
         <v>64</v>
-      </c>
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" t="s">
-        <v>65</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -953,22 +968,66 @@
       <c r="B23" t="s">
         <v>25</v>
       </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23">
+        <v>9</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>11</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>23</v>
       </c>
-      <c r="C24" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24">
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26">
         <v>1E+18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>